<commit_message>
split excel file into two
</commit_message>
<xml_diff>
--- a/Paulsen/Microsatellite genotype data.xlsx
+++ b/Paulsen/Microsatellite genotype data.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muras\Documents\R\BCB546X_Final_Project\Paulsen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B501C1B-FE59-4D90-ABCE-1D2BE52E8706}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="19395" windowHeight="7605"/>
+    <workbookView minimized="1" xWindow="600" yWindow="110" windowWidth="19400" windowHeight="7610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microsatellite genotype data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sampling information" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="239">
   <si>
     <t>sha1</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -767,652 +772,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>population</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Individual ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Population</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Original code</t>
-  </si>
-  <si>
-    <t>XG1</t>
-  </si>
-  <si>
-    <t>ZWY-A2</t>
-  </si>
-  <si>
-    <t>ZWY-S2</t>
-  </si>
-  <si>
-    <t>ZWY-S3</t>
-  </si>
-  <si>
-    <t>ZWY-S4</t>
-  </si>
-  <si>
-    <t>ZWY-S5</t>
-  </si>
-  <si>
-    <t>NN-A1</t>
-  </si>
-  <si>
-    <t>NN-A2</t>
-  </si>
-  <si>
-    <t>NN-A3</t>
-  </si>
-  <si>
-    <t>NN-A4</t>
-  </si>
-  <si>
-    <t>NN-A5</t>
-  </si>
-  <si>
-    <t>DA-9</t>
-  </si>
-  <si>
-    <t>DA-10</t>
-  </si>
-  <si>
-    <t>DA-11</t>
-  </si>
-  <si>
-    <t>DA-21</t>
-  </si>
-  <si>
-    <t>ND-A1</t>
-  </si>
-  <si>
-    <t>ND-A3</t>
-  </si>
-  <si>
-    <t>ND-7.1</t>
-  </si>
-  <si>
-    <t>ND-8.6</t>
-  </si>
-  <si>
-    <t>ND-10.1</t>
-  </si>
-  <si>
-    <t>ND-9.13</t>
-  </si>
-  <si>
-    <t>ND-8.1</t>
-  </si>
-  <si>
-    <t>ND-11.1</t>
-  </si>
-  <si>
-    <t>ND-3.4</t>
-  </si>
-  <si>
-    <t>ND-3.3</t>
-  </si>
-  <si>
-    <t>ND-4.1</t>
-  </si>
-  <si>
-    <t>ND-2.8</t>
-  </si>
-  <si>
-    <t>ND-2.5</t>
-  </si>
-  <si>
-    <t>ND-6.1</t>
-  </si>
-  <si>
-    <t>ND-6.2</t>
-  </si>
-  <si>
-    <t>ND-8.2</t>
-  </si>
-  <si>
-    <t>ND-3.5</t>
-  </si>
-  <si>
-    <t>ND-8.3</t>
-  </si>
-  <si>
-    <t>ND-8.4</t>
-  </si>
-  <si>
-    <t>ND-8.8</t>
-  </si>
-  <si>
-    <t>sha-1.5</t>
-  </si>
-  <si>
-    <t>sha-2.1</t>
-  </si>
-  <si>
-    <t>sha-2.2</t>
-  </si>
-  <si>
-    <t>sha-3.1</t>
-  </si>
-  <si>
-    <t>sha-4.1</t>
-  </si>
-  <si>
-    <t>sha-4.2</t>
-  </si>
-  <si>
-    <t>sha-4.3</t>
-  </si>
-  <si>
-    <t>sha-5.2</t>
-  </si>
-  <si>
-    <t>sha-5.3</t>
-  </si>
-  <si>
-    <t>sha-6.1</t>
-  </si>
-  <si>
-    <t>sha-6.3</t>
-  </si>
-  <si>
-    <t>sha-7.1</t>
-  </si>
-  <si>
-    <t>sha-8.1</t>
-  </si>
-  <si>
-    <t>sha-8.2</t>
-  </si>
-  <si>
-    <t>sha-8.9</t>
-  </si>
-  <si>
-    <t>sha-A</t>
-  </si>
-  <si>
-    <t>sha-B</t>
-  </si>
-  <si>
-    <t>sha-B1</t>
-  </si>
-  <si>
-    <t>sha-C</t>
-  </si>
-  <si>
-    <t>sha-C1</t>
-  </si>
-  <si>
-    <t>sha-D</t>
-  </si>
-  <si>
-    <t>sha-D1</t>
-  </si>
-  <si>
-    <t>sha-E</t>
-  </si>
-  <si>
-    <t>sha-F</t>
-  </si>
-  <si>
-    <t>sha-G</t>
-  </si>
-  <si>
-    <t>sha-H</t>
-  </si>
-  <si>
-    <t>sha-I</t>
-  </si>
-  <si>
-    <t>JX-4.1</t>
-  </si>
-  <si>
-    <t>JX-4.17</t>
-  </si>
-  <si>
-    <t>JX-5.12</t>
-  </si>
-  <si>
-    <t>JX-6.5</t>
-  </si>
-  <si>
-    <t>JX-7.1</t>
-  </si>
-  <si>
-    <t>JX-8.3</t>
-  </si>
-  <si>
-    <t>JX-13.1</t>
-  </si>
-  <si>
-    <t>JX-14.4</t>
-  </si>
-  <si>
-    <t>JX-15.4</t>
-  </si>
-  <si>
-    <t>JX-10.1</t>
-  </si>
-  <si>
-    <t>JX-10.2</t>
-  </si>
-  <si>
-    <t>JX-10.8</t>
-  </si>
-  <si>
-    <t>JX-16.4</t>
-  </si>
-  <si>
-    <t>JX-17.1</t>
-  </si>
-  <si>
-    <t>JX-18.1</t>
-  </si>
-  <si>
-    <t>JX-4.9</t>
-  </si>
-  <si>
-    <t>JX-6.3</t>
-  </si>
-  <si>
-    <t>JX-6.4</t>
-  </si>
-  <si>
-    <t>JX-8.2</t>
-  </si>
-  <si>
-    <t>JX-8.7</t>
-  </si>
-  <si>
-    <t>ZWY-A1</t>
-  </si>
-  <si>
-    <t>ZWY-B</t>
-  </si>
-  <si>
-    <t>ZWY-C1</t>
-  </si>
-  <si>
-    <t>ZWY-D1</t>
-  </si>
-  <si>
-    <t>ZWY-I</t>
-  </si>
-  <si>
-    <t>ZWY-S1</t>
-  </si>
-  <si>
-    <t>ZWY-S11</t>
-  </si>
-  <si>
-    <t>ZWY-S13</t>
-  </si>
-  <si>
-    <t>ZWY-E1</t>
-  </si>
-  <si>
-    <t>ZWY-E2</t>
-  </si>
-  <si>
-    <t>DHS-AA-1</t>
-  </si>
-  <si>
-    <t>DHS-BB-1</t>
-  </si>
-  <si>
-    <t>DHS-CC-1</t>
-  </si>
-  <si>
-    <t>DHS-DD-1</t>
-  </si>
-  <si>
-    <t>DHS-C-1</t>
-  </si>
-  <si>
-    <t>DHS-E-1</t>
-  </si>
-  <si>
-    <t>DHS-G-1</t>
-  </si>
-  <si>
-    <t>DHS-A-1</t>
-  </si>
-  <si>
-    <t>DHS-W-1</t>
-  </si>
-  <si>
-    <t>DHS-Y-1</t>
-  </si>
-  <si>
-    <t>DHS-YK-A1</t>
-  </si>
-  <si>
-    <t>DHS-YK-B1</t>
-  </si>
-  <si>
-    <t>DHS-YK-C1</t>
-  </si>
-  <si>
-    <t>DHS-YK-D1</t>
-  </si>
-  <si>
-    <t>DHS-YK-A2</t>
-  </si>
-  <si>
-    <t>DHS-YK-C2</t>
-  </si>
-  <si>
-    <t>DHS-YK-D2</t>
-  </si>
-  <si>
-    <t>DHS-YK-E1</t>
-  </si>
-  <si>
-    <t>DHS-YK-E2</t>
-  </si>
-  <si>
-    <t>DHS-YK-H1</t>
-  </si>
-  <si>
-    <t>DHS-YK-I1</t>
-  </si>
-  <si>
-    <t>DHS-YK-J1</t>
-  </si>
-  <si>
-    <t>DHS-YK-B2</t>
-  </si>
-  <si>
-    <t>DHS-YK-J2</t>
-  </si>
-  <si>
-    <t>HN11.2</t>
-  </si>
-  <si>
-    <t>HN11.1</t>
-  </si>
-  <si>
-    <t>HN11.4</t>
-  </si>
-  <si>
-    <t>HN11.3</t>
-  </si>
-  <si>
-    <t>HN10.2</t>
-  </si>
-  <si>
-    <t>HN-A</t>
-  </si>
-  <si>
-    <t>HN-B</t>
-  </si>
-  <si>
-    <t>HN-C</t>
-  </si>
-  <si>
-    <t>HN-D</t>
-  </si>
-  <si>
-    <t>HN-E</t>
-  </si>
-  <si>
-    <t>HN-F</t>
-  </si>
-  <si>
-    <t>HN-G</t>
-  </si>
-  <si>
-    <t>HN-H</t>
-  </si>
-  <si>
-    <t>HN-I</t>
-  </si>
-  <si>
-    <t>HN-J</t>
-  </si>
-  <si>
-    <t>HN-K</t>
-  </si>
-  <si>
-    <t>HN-L</t>
-  </si>
-  <si>
-    <t>SD1</t>
-  </si>
-  <si>
-    <t>NN-3</t>
-  </si>
-  <si>
-    <t>NN-16</t>
-  </si>
-  <si>
-    <t>NN-9</t>
-  </si>
-  <si>
-    <t>NN-7</t>
-  </si>
-  <si>
-    <t>NN-10</t>
-  </si>
-  <si>
-    <t>NN-8</t>
-  </si>
-  <si>
-    <t>NN-5</t>
-  </si>
-  <si>
-    <t>NN-15</t>
-  </si>
-  <si>
-    <t>NN-11</t>
-  </si>
-  <si>
-    <t>NN-13</t>
-  </si>
-  <si>
-    <t>NN-14</t>
-  </si>
-  <si>
-    <t>NN-2</t>
-  </si>
-  <si>
-    <t>NN-4</t>
-  </si>
-  <si>
-    <t>NN-1</t>
-  </si>
-  <si>
-    <t>DA-1</t>
-  </si>
-  <si>
-    <t>DA-5</t>
-  </si>
-  <si>
-    <t>DA-6</t>
-  </si>
-  <si>
-    <t>DA-8</t>
-  </si>
-  <si>
-    <t>DA-16</t>
-  </si>
-  <si>
-    <t>DA-20</t>
-  </si>
-  <si>
-    <t>DA-23</t>
-  </si>
-  <si>
-    <t>DA-62</t>
-  </si>
-  <si>
-    <t>DA-61</t>
-  </si>
-  <si>
-    <t>DA-60</t>
-  </si>
-  <si>
-    <t>DA-58</t>
-  </si>
-  <si>
-    <t>DA-57</t>
-  </si>
-  <si>
-    <t>DA-55</t>
-  </si>
-  <si>
-    <t>DA-53</t>
-  </si>
-  <si>
-    <t>DA-51</t>
-  </si>
-  <si>
-    <t>WN1</t>
-  </si>
-  <si>
-    <t>XG822-13-）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG837-44-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG826-19-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG836-42-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG837-44-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG827-4-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG836-10-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG837-44-10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XG827-23-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1426,21 +816,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1480,7 +870,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1520,12 +910,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1534,11 +921,19 @@
       <color rgb="FFFF0066"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1580,7 +975,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1612,9 +1007,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1646,6 +1059,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1821,16 +1252,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -1920,10 +1351,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>215</v>
@@ -3264,7 +2695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="14.25">
+    <row r="25" spans="1:21" ht="15">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -3389,7 +2820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="14.25">
+    <row r="27" spans="1:21" ht="15">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -3575,7 +3006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="14.25">
+    <row r="30" spans="1:21" ht="15">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -3637,7 +3068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="14.25">
+    <row r="31" spans="1:21" ht="15">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
@@ -3699,7 +3130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="14.25">
+    <row r="32" spans="1:21" ht="15">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -3761,7 +3192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="14.25">
+    <row r="33" spans="1:20" ht="15">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -3823,7 +3254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.25">
+    <row r="34" spans="1:20" ht="15">
       <c r="A34" s="2" t="s">
         <v>10</v>
       </c>
@@ -3885,7 +3316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="14.25">
+    <row r="35" spans="1:20" ht="15">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -3947,7 +3378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="14.25">
+    <row r="36" spans="1:20" ht="15">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -4009,7 +3440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="14.25">
+    <row r="37" spans="1:20" ht="15">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -4071,7 +3502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="14.25">
+    <row r="38" spans="1:20" ht="15">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -4195,7 +3626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="14.25">
+    <row r="40" spans="1:20" ht="15">
       <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
@@ -4257,7 +3688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="14.25">
+    <row r="41" spans="1:20" ht="15">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
@@ -4319,7 +3750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="14.25">
+    <row r="42" spans="1:20" ht="15">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -4381,7 +3812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="14.25">
+    <row r="43" spans="1:20" ht="15">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -4443,7 +3874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="14.25">
+    <row r="44" spans="1:20" ht="15">
       <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
@@ -4505,7 +3936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="14.25">
+    <row r="45" spans="1:20" ht="15">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
@@ -4567,7 +3998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="14.25">
+    <row r="46" spans="1:20" ht="15">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
@@ -4629,7 +4060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="14.25">
+    <row r="47" spans="1:20" ht="15">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -4691,7 +4122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="14.25">
+    <row r="48" spans="1:20" ht="15">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
@@ -4753,7 +4184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="14.25">
+    <row r="49" spans="1:20" ht="15">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -4815,7 +4246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="14.25">
+    <row r="50" spans="1:20" ht="15">
       <c r="A50" s="2" t="s">
         <v>26</v>
       </c>
@@ -14864,2949 +14295,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D209"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="15">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="15">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>280</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="15">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>281</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="15">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="15">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="15">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>284</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="15">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>285</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="15">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>286</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="15">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="15">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>288</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="15">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>289</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="15">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="15">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>291</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="15">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>292</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="15">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>293</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="15">
-        <v>8</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>294</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="15">
-        <v>8</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>295</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="15">
-        <v>8</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="15">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>297</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="15">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>298</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="15">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>299</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="15">
-        <v>3</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="15">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>301</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="15">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>302</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="15">
-        <v>4</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>303</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="15">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>304</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="15">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>305</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="15">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>306</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="15">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>307</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="15">
-        <v>7</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>308</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="15">
-        <v>8</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>309</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="15">
-        <v>8</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>310</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="15">
-        <v>8</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>311</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>312</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>313</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>314</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>315</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>316</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>317</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>318</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>319</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>320</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>321</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>322</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>323</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="15">
-        <v>4</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>324</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="15">
-        <v>4</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>325</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="15">
-        <v>5</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>326</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="15">
-        <v>6</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
-        <v>327</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" s="15">
-        <v>7</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>328</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="15">
-        <v>8</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>329</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="15">
-        <v>13</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>330</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="15">
-        <v>14</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>331</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="15">
-        <v>15</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>332</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="15">
-        <v>10</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>333</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="15">
-        <v>10</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>334</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="15">
-        <v>10</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>335</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" s="15">
-        <v>16</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" t="s">
-        <v>336</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="15">
-        <v>17</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
-        <v>337</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" s="15">
-        <v>18</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>338</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="15">
-        <v>4</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" t="s">
-        <v>339</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="15">
-        <v>6</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>340</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C66" s="15">
-        <v>6</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>341</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="15">
-        <v>8</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>342</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C68" s="15">
-        <v>8</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>261</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" t="s">
-        <v>425</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70" s="15">
-        <v>822</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" t="s">
-        <v>426</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71" s="15">
-        <v>837</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" t="s">
-        <v>427</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C72" s="15">
-        <v>826</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" t="s">
-        <v>428</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="15">
-        <v>836</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" t="s">
-        <v>33</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
-        <v>429</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="15">
-        <v>837</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
-        <v>35</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
-        <v>430</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="15">
-        <v>827</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" t="s">
-        <v>38</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" t="s">
-        <v>431</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C80" s="15">
-        <v>836</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
-        <v>432</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C81" s="15">
-        <v>837</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
-        <v>41</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
-        <v>433</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C83" s="15">
-        <v>827</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" t="s">
-        <v>43</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" t="s">
-        <v>343</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" t="s">
-        <v>262</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
-        <v>344</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" t="s">
-        <v>345</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" t="s">
-        <v>346</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" t="s">
-        <v>347</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" t="s">
-        <v>348</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" t="s">
-        <v>263</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
-        <v>264</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
-        <v>265</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" t="s">
-        <v>266</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" t="s">
-        <v>349</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" t="s">
-        <v>350</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" t="s">
-        <v>351</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" t="s">
-        <v>352</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
-        <v>353</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" t="s">
-        <v>354</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
-      <c r="A102" t="s">
-        <v>355</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
-      <c r="A103" t="s">
-        <v>356</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" t="s">
-        <v>357</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
-      <c r="A105" t="s">
-        <v>358</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" t="s">
-        <v>359</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" t="s">
-        <v>360</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" t="s">
-        <v>361</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
-      <c r="A109" t="s">
-        <v>362</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" t="s">
-        <v>363</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" t="s">
-        <v>364</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" t="s">
-        <v>365</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" t="s">
-        <v>366</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" t="s">
-        <v>367</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" t="s">
-        <v>368</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" t="s">
-        <v>369</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" t="s">
-        <v>370</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" t="s">
-        <v>371</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" t="s">
-        <v>372</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" t="s">
-        <v>373</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" t="s">
-        <v>374</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" t="s">
-        <v>375</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C122" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" t="s">
-        <v>376</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="D123" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" t="s">
-        <v>377</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C124" s="15">
-        <v>11</v>
-      </c>
-      <c r="D124" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" t="s">
-        <v>110</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C125" s="15">
-        <v>8</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" t="s">
-        <v>378</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C126" s="15">
-        <v>11</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" t="s">
-        <v>379</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C127" s="15">
-        <v>11</v>
-      </c>
-      <c r="D127" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
-      <c r="A128" t="s">
-        <v>380</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C128" s="15">
-        <v>11</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="A129" t="s">
-        <v>106</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C129" s="15">
-        <v>4</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" t="s">
-        <v>112</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C130" s="15">
-        <v>10</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" t="s">
-        <v>381</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C131" s="15">
-        <v>10</v>
-      </c>
-      <c r="D131" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132" t="s">
-        <v>382</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D132" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" t="s">
-        <v>383</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C133" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D133" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" t="s">
-        <v>384</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C134" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D134" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" t="s">
-        <v>385</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C135" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" t="s">
-        <v>386</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" t="s">
-        <v>387</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C137" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D137" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" t="s">
-        <v>388</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C138" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" t="s">
-        <v>389</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140" t="s">
-        <v>390</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C140" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141" t="s">
-        <v>391</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C141" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D141" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" t="s">
-        <v>392</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C142" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" t="s">
-        <v>393</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C143" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D143" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" t="s">
-        <v>394</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C144" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="A145" t="s">
-        <v>87</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C145" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146" t="s">
-        <v>88</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C146" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D146" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
-      <c r="A147" t="s">
-        <v>89</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C147" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148" t="s">
-        <v>90</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D148" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149" t="s">
-        <v>91</v>
-      </c>
-      <c r="B149" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" t="s">
-        <v>92</v>
-      </c>
-      <c r="B150" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C150" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D150" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="A151" t="s">
-        <v>93</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C151" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D151" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="A152" t="s">
-        <v>94</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C152" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D152" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="A153" t="s">
-        <v>95</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C153" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="A154" t="s">
-        <v>96</v>
-      </c>
-      <c r="B154" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C154" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155" t="s">
-        <v>97</v>
-      </c>
-      <c r="B155" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C155" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D155" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="A156" t="s">
-        <v>98</v>
-      </c>
-      <c r="B156" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C156" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D156" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="A157" t="s">
-        <v>99</v>
-      </c>
-      <c r="B157" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C157" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D157" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" t="s">
-        <v>100</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C158" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" t="s">
-        <v>101</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C159" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160" t="s">
-        <v>102</v>
-      </c>
-      <c r="B160" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C160" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="A161" t="s">
-        <v>103</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C161" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D161" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
-      <c r="A162" t="s">
-        <v>395</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C162" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D162" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
-      <c r="A163" t="s">
-        <v>396</v>
-      </c>
-      <c r="B163" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D163" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
-      <c r="A164" t="s">
-        <v>397</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C164" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
-      <c r="A165" t="s">
-        <v>398</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C165" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D165" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
-      <c r="A166" t="s">
-        <v>399</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C166" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
-      <c r="A167" t="s">
-        <v>400</v>
-      </c>
-      <c r="B167" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C167" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
-      <c r="A168" t="s">
-        <v>401</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C168" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="A169" t="s">
-        <v>402</v>
-      </c>
-      <c r="B169" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C169" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="A170" t="s">
-        <v>403</v>
-      </c>
-      <c r="B170" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C170" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="A171" t="s">
-        <v>404</v>
-      </c>
-      <c r="B171" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C171" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="A172" t="s">
-        <v>405</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C172" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D172" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
-      <c r="A173" t="s">
-        <v>406</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C173" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D173" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174" t="s">
-        <v>407</v>
-      </c>
-      <c r="B174" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C174" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
-      <c r="A175" t="s">
-        <v>408</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C175" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D175" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
-      <c r="A176" t="s">
-        <v>267</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C176" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D176" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4">
-      <c r="A177" t="s">
-        <v>268</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C177" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D177" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
-      <c r="A178" t="s">
-        <v>269</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D178" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4">
-      <c r="A179" t="s">
-        <v>270</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C179" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D179" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4">
-      <c r="A180" t="s">
-        <v>271</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C180" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D180" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
-      <c r="A181" t="s">
-        <v>409</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C181" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D181" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
-      <c r="A182" t="s">
-        <v>410</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C182" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D182" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="A183" t="s">
-        <v>411</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C183" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D183" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="A184" t="s">
-        <v>412</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C184" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D184" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
-      <c r="A185" t="s">
-        <v>272</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C185" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D185" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
-      <c r="A186" t="s">
-        <v>273</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C186" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D186" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
-      <c r="A187" t="s">
-        <v>274</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C187" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D187" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" t="s">
-        <v>413</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C188" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D188" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" t="s">
-        <v>414</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C189" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D189" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
-      <c r="A190" t="s">
-        <v>275</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C190" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D190" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" t="s">
-        <v>415</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C191" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
-      <c r="A192" t="s">
-        <v>416</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C192" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
-      <c r="A193" t="s">
-        <v>417</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C193" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
-      <c r="A194" t="s">
-        <v>418</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C194" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D194" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4">
-      <c r="A195" t="s">
-        <v>419</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C195" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4">
-      <c r="A196" t="s">
-        <v>420</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C196" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="A197" t="s">
-        <v>421</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C197" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4">
-      <c r="A198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C198" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D198" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4">
-      <c r="A199" t="s">
-        <v>423</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C199" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4">
-      <c r="A200" t="s">
-        <v>424</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C200" s="15">
-        <v>1</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4">
-      <c r="A201" t="s">
-        <v>204</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C201" s="15">
-        <v>1</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4">
-      <c r="A202" t="s">
-        <v>205</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C202" s="15">
-        <v>1</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" t="s">
-        <v>206</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C203" s="15">
-        <v>1</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="A204" t="s">
-        <v>207</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C204" s="15">
-        <v>1</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
-      <c r="A205" t="s">
-        <v>208</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C205" s="15">
-        <v>1</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4">
-      <c r="A206" t="s">
-        <v>209</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C206" s="15">
-        <v>1</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" t="s">
-        <v>210</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C207" s="15">
-        <v>1</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4">
-      <c r="A208" t="s">
-        <v>211</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C208" s="15">
-        <v>1</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4">
-      <c r="A209" t="s">
-        <v>212</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C209" s="15">
-        <v>1</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>